<commit_message>
login, register, jwt verifciation
</commit_message>
<xml_diff>
--- a/Docs/password.xlsx
+++ b/Docs/password.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F19887-5767-46E4-93E4-B237ED1A5F12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A475C9F6-1AD4-4D25-863B-B40E3957960C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,7 +361,7 @@
   <dimension ref="D2:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>